<commit_message>
added saving to formatted file
</commit_message>
<xml_diff>
--- a/irena_cap_summary.xlsx
+++ b/irena_cap_summary.xlsx
@@ -7,13 +7,13 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Solar photovoltaic" sheetId="1" r:id="rId1"/>
-    <sheet name="Pumped storage" sheetId="2" r:id="rId2"/>
+    <sheet name="Mixed Hydro Plants" sheetId="1" r:id="rId1"/>
+    <sheet name="Offshore wind energy" sheetId="2" r:id="rId2"/>
     <sheet name="Renewable hydropower" sheetId="3" r:id="rId3"/>
     <sheet name="Onshore wind energy" sheetId="4" r:id="rId4"/>
-    <sheet name="Mixed Hydro Plants" sheetId="5" r:id="rId5"/>
-    <sheet name="Concentrated solar power" sheetId="6" r:id="rId6"/>
-    <sheet name="Offshore wind energy" sheetId="7" r:id="rId7"/>
+    <sheet name="Concentrated solar power" sheetId="5" r:id="rId5"/>
+    <sheet name="Pumped storage" sheetId="6" r:id="rId6"/>
+    <sheet name="Solar photovoltaic" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -492,7 +492,7 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>3937</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -503,7 +503,7 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>16.02</v>
+        <v>27.63000000000011</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -514,7 +514,7 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>67.8</v>
+        <v>827.8900000000003</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -525,7 +525,7 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>848.28</v>
+        <v>400.8699999999999</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -536,7 +536,7 @@
         <v>2020</v>
       </c>
       <c r="C6">
-        <v>1283</v>
+        <v>812.8899999999994</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -558,7 +558,7 @@
         <v>2005</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -569,7 +569,7 @@
         <v>2010</v>
       </c>
       <c r="C9">
-        <v>1004.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -580,7 +580,7 @@
         <v>2015</v>
       </c>
       <c r="C10">
-        <v>2125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -591,7 +591,7 @@
         <v>2020</v>
       </c>
       <c r="C11">
-        <v>2514.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -602,7 +602,7 @@
         <v>2000</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -624,7 +624,7 @@
         <v>2010</v>
       </c>
       <c r="C14">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -635,7 +635,7 @@
         <v>2015</v>
       </c>
       <c r="C15">
-        <v>1004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -646,7 +646,7 @@
         <v>2020</v>
       </c>
       <c r="C16">
-        <v>43.95000000000005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -657,7 +657,7 @@
         <v>2000</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>275.4</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -679,7 +679,7 @@
         <v>2010</v>
       </c>
       <c r="C19">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -690,7 +690,7 @@
         <v>2015</v>
       </c>
       <c r="C20">
-        <v>47.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -701,7 +701,7 @@
         <v>2020</v>
       </c>
       <c r="C21">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -712,7 +712,7 @@
         <v>2000</v>
       </c>
       <c r="C22">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -723,7 +723,7 @@
         <v>2005</v>
       </c>
       <c r="C23">
-        <v>0.49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -734,7 +734,7 @@
         <v>2010</v>
       </c>
       <c r="C24">
-        <v>1726.41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -745,7 +745,7 @@
         <v>2015</v>
       </c>
       <c r="C25">
-        <v>346.4200000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -767,7 +767,7 @@
         <v>2000</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -778,7 +778,7 @@
         <v>2005</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -789,7 +789,7 @@
         <v>2010</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -800,7 +800,7 @@
         <v>2015</v>
       </c>
       <c r="C30">
-        <v>775.11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -811,7 +811,7 @@
         <v>2020</v>
       </c>
       <c r="C31">
-        <v>517.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -844,7 +844,7 @@
         <v>2010</v>
       </c>
       <c r="C34">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -855,7 +855,7 @@
         <v>2015</v>
       </c>
       <c r="C35">
-        <v>6.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -866,7 +866,7 @@
         <v>2020</v>
       </c>
       <c r="C36">
-        <v>123.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -877,7 +877,7 @@
         <v>2000</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -888,7 +888,7 @@
         <v>2005</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -899,7 +899,7 @@
         <v>2010</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -910,7 +910,7 @@
         <v>2015</v>
       </c>
       <c r="C40">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -921,7 +921,7 @@
         <v>2020</v>
       </c>
       <c r="C41">
-        <v>374</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -932,7 +932,7 @@
         <v>2000</v>
       </c>
       <c r="C42">
-        <v>7</v>
+        <v>5408.63</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -943,7 +943,7 @@
         <v>2005</v>
       </c>
       <c r="C43">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -954,7 +954,7 @@
         <v>2010</v>
       </c>
       <c r="C44">
-        <v>1031</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -965,7 +965,7 @@
         <v>2015</v>
       </c>
       <c r="C45">
-        <v>6093.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -976,7 +976,7 @@
         <v>2020</v>
       </c>
       <c r="C46">
-        <v>4586.93</v>
+        <v>85.59999999999945</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -987,7 +987,7 @@
         <v>2000</v>
       </c>
       <c r="C47">
-        <v>114</v>
+        <v>745</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -998,7 +998,7 @@
         <v>2005</v>
       </c>
       <c r="C48">
-        <v>1942</v>
+        <v>331</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1009,7 +1009,7 @@
         <v>2010</v>
       </c>
       <c r="C49">
-        <v>15948</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1020,7 +1020,7 @@
         <v>2015</v>
       </c>
       <c r="C50">
-        <v>21218</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1031,7 +1031,7 @@
         <v>2020</v>
       </c>
       <c r="C51">
-        <v>14559</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1042,7 +1042,7 @@
         <v>2000</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>699</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1053,7 +1053,7 @@
         <v>2005</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1064,7 +1064,7 @@
         <v>2010</v>
       </c>
       <c r="C54">
-        <v>201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1075,7 +1075,7 @@
         <v>2015</v>
       </c>
       <c r="C55">
-        <v>2402</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1086,7 +1086,7 @@
         <v>2020</v>
       </c>
       <c r="C56">
-        <v>643</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1119,7 +1119,7 @@
         <v>2010</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1130,7 +1130,7 @@
         <v>2015</v>
       </c>
       <c r="C60">
-        <v>170</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1141,7 +1141,7 @@
         <v>2020</v>
       </c>
       <c r="C61">
-        <v>1781</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1174,7 +1174,7 @@
         <v>2010</v>
       </c>
       <c r="C64">
-        <v>0.6899999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1185,7 +1185,7 @@
         <v>2015</v>
       </c>
       <c r="C65">
-        <v>1.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1196,7 +1196,7 @@
         <v>2020</v>
       </c>
       <c r="C66">
-        <v>37.84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1207,7 +1207,7 @@
         <v>2000</v>
       </c>
       <c r="C67">
-        <v>19</v>
+        <v>3001</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1218,7 +1218,7 @@
         <v>2005</v>
       </c>
       <c r="C68">
-        <v>15</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1229,7 +1229,7 @@
         <v>2010</v>
       </c>
       <c r="C69">
-        <v>3558</v>
+        <v>157.6100000000001</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1240,7 +1240,7 @@
         <v>2015</v>
       </c>
       <c r="C70">
-        <v>15309</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1251,7 +1251,7 @@
         <v>2020</v>
       </c>
       <c r="C71">
-        <v>2693.279999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1295,7 +1295,7 @@
         <v>2015</v>
       </c>
       <c r="C75">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1306,7 +1306,7 @@
         <v>2020</v>
       </c>
       <c r="C76">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1339,7 +1339,7 @@
         <v>2010</v>
       </c>
       <c r="C79">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1350,7 +1350,7 @@
         <v>2015</v>
       </c>
       <c r="C80">
-        <v>68.90000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1361,7 +1361,7 @@
         <v>2020</v>
       </c>
       <c r="C81">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1383,7 +1383,7 @@
         <v>2005</v>
       </c>
       <c r="C83">
-        <v>23.58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1394,7 +1394,7 @@
         <v>2010</v>
       </c>
       <c r="C84">
-        <v>5.870000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1405,7 +1405,7 @@
         <v>2015</v>
       </c>
       <c r="C85">
-        <v>86.81999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1416,7 +1416,7 @@
         <v>2020</v>
       </c>
       <c r="C86">
-        <v>78.47000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1427,7 +1427,7 @@
         <v>2000</v>
       </c>
       <c r="C87">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1438,7 +1438,7 @@
         <v>2005</v>
       </c>
       <c r="C88">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1449,7 +1449,7 @@
         <v>2010</v>
       </c>
       <c r="C89">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1460,7 +1460,7 @@
         <v>2015</v>
       </c>
       <c r="C90">
-        <v>1436</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1471,7 +1471,7 @@
         <v>2020</v>
       </c>
       <c r="C91">
-        <v>8687</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1482,7 +1482,7 @@
         <v>2000</v>
       </c>
       <c r="C92">
-        <v>6</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1493,7 +1493,7 @@
         <v>2005</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1504,7 +1504,7 @@
         <v>2010</v>
       </c>
       <c r="C94">
-        <v>2.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1515,7 +1515,7 @@
         <v>2015</v>
       </c>
       <c r="C95">
-        <v>5.9</v>
+        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1526,7 +1526,7 @@
         <v>2020</v>
       </c>
       <c r="C96">
-        <v>136.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1537,7 +1537,7 @@
         <v>2000</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>308</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1548,7 +1548,7 @@
         <v>2005</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1559,7 +1559,7 @@
         <v>2010</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>2.949999999999989</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1570,7 +1570,7 @@
         <v>2015</v>
       </c>
       <c r="C100">
-        <v>107.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1581,7 +1581,7 @@
         <v>2020</v>
       </c>
       <c r="C101">
-        <v>3827.96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1592,7 +1592,7 @@
         <v>2000</v>
       </c>
       <c r="C102">
-        <v>1</v>
+        <v>617</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1603,7 +1603,7 @@
         <v>2005</v>
       </c>
       <c r="C103">
-        <v>1</v>
+        <v>431.9000000000001</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1614,7 +1614,7 @@
         <v>2010</v>
       </c>
       <c r="C104">
-        <v>132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1625,7 +1625,7 @@
         <v>2015</v>
       </c>
       <c r="C105">
-        <v>313</v>
+        <v>673.0999999999999</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -1636,7 +1636,7 @@
         <v>2020</v>
       </c>
       <c r="C106">
-        <v>578.4400000000001</v>
+        <v>1042.4</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1669,7 +1669,7 @@
         <v>2010</v>
       </c>
       <c r="C109">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -1680,7 +1680,7 @@
         <v>2015</v>
       </c>
       <c r="C110">
-        <v>1325.9</v>
+        <v>278.25</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1691,7 +1691,7 @@
         <v>2020</v>
       </c>
       <c r="C111">
-        <v>60.71000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -1724,7 +1724,7 @@
         <v>2010</v>
       </c>
       <c r="C114">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -1735,7 +1735,7 @@
         <v>2015</v>
       </c>
       <c r="C115">
-        <v>514</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1746,7 +1746,7 @@
         <v>2020</v>
       </c>
       <c r="C116">
-        <v>59.89999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -1757,7 +1757,7 @@
         <v>2000</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1779,7 +1779,7 @@
         <v>2010</v>
       </c>
       <c r="C119">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1790,7 +1790,7 @@
         <v>2015</v>
       </c>
       <c r="C120">
-        <v>226</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1801,7 +1801,7 @@
         <v>2020</v>
       </c>
       <c r="C121">
-        <v>28.81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1812,7 +1812,7 @@
         <v>2000</v>
       </c>
       <c r="C122">
-        <v>10</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -1823,7 +1823,7 @@
         <v>2005</v>
       </c>
       <c r="C123">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -1834,7 +1834,7 @@
         <v>2010</v>
       </c>
       <c r="C124">
-        <v>3821</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -1845,7 +1845,7 @@
         <v>2015</v>
       </c>
       <c r="C125">
-        <v>831</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -1856,7 +1856,7 @@
         <v>2020</v>
       </c>
       <c r="C126">
-        <v>7081.01</v>
+        <v>303</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -1867,7 +1867,7 @@
         <v>2000</v>
       </c>
       <c r="C127">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -1878,7 +1878,7 @@
         <v>2005</v>
       </c>
       <c r="C128">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -1889,7 +1889,7 @@
         <v>2010</v>
       </c>
       <c r="C129">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -1900,7 +1900,7 @@
         <v>2015</v>
       </c>
       <c r="C130">
-        <v>93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -1911,7 +1911,7 @@
         <v>2020</v>
       </c>
       <c r="C131">
-        <v>1313.15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1922,7 +1922,7 @@
         <v>2000</v>
       </c>
       <c r="C132">
-        <v>16</v>
+        <v>9288</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -1933,7 +1933,7 @@
         <v>2005</v>
       </c>
       <c r="C133">
-        <v>12</v>
+        <v>62</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -1944,7 +1944,7 @@
         <v>2010</v>
       </c>
       <c r="C134">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1955,7 +1955,7 @@
         <v>2015</v>
       </c>
       <c r="C135">
-        <v>1269</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -1966,7 +1966,7 @@
         <v>2020</v>
       </c>
       <c r="C136">
-        <v>1549.25</v>
+        <v>1467</v>
       </c>
     </row>
   </sheetData>
@@ -2056,7 +2056,7 @@
         <v>2000</v>
       </c>
       <c r="C7">
-        <v>1307</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2078,7 +2078,7 @@
         <v>2010</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>196.5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2089,7 +2089,7 @@
         <v>2015</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>515.5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2100,7 +2100,7 @@
         <v>2020</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1541.9</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2111,7 +2111,7 @@
         <v>2000</v>
       </c>
       <c r="C12">
-        <v>864</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2221,7 +2221,7 @@
         <v>2000</v>
       </c>
       <c r="C22">
-        <v>1145</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2232,7 +2232,7 @@
         <v>2005</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2254,7 +2254,7 @@
         <v>2015</v>
       </c>
       <c r="C25">
-        <v>24.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2276,7 +2276,7 @@
         <v>2000</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>49.95</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2287,7 +2287,7 @@
         <v>2005</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>373.4</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2298,7 +2298,7 @@
         <v>2010</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>444.5</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2309,7 +2309,7 @@
         <v>2015</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>403.1999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2320,7 +2320,7 @@
         <v>2020</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>429.75</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2408,7 +2408,7 @@
         <v>2010</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>26.3</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2419,7 +2419,7 @@
         <v>2015</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>5.699999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2430,7 +2430,7 @@
         <v>2020</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2441,7 +2441,7 @@
         <v>2000</v>
       </c>
       <c r="C42">
-        <v>1727.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2485,7 +2485,7 @@
         <v>2020</v>
       </c>
       <c r="C46">
-        <v>0.03999999999996362</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2496,7 +2496,7 @@
         <v>2000</v>
       </c>
       <c r="C47">
-        <v>4654</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2507,7 +2507,7 @@
         <v>2005</v>
       </c>
       <c r="C48">
-        <v>701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2518,7 +2518,7 @@
         <v>2010</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2529,7 +2529,7 @@
         <v>2015</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>3203</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2540,7 +2540,7 @@
         <v>2020</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2672,7 +2672,7 @@
         <v>2005</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2694,7 +2694,7 @@
         <v>2015</v>
       </c>
       <c r="C65">
-        <v>292</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2716,7 +2716,7 @@
         <v>2000</v>
       </c>
       <c r="C67">
-        <v>3940.38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2826,7 +2826,7 @@
         <v>2000</v>
       </c>
       <c r="C77">
-        <v>760</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2881,7 +2881,7 @@
         <v>2000</v>
       </c>
       <c r="C82">
-        <v>1100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2914,7 +2914,7 @@
         <v>2015</v>
       </c>
       <c r="C85">
-        <v>196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2958,7 +2958,7 @@
         <v>2010</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>228</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2969,7 +2969,7 @@
         <v>2015</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>129</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2980,7 +2980,7 @@
         <v>2020</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -3013,7 +3013,7 @@
         <v>2010</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -3046,7 +3046,7 @@
         <v>2000</v>
       </c>
       <c r="C97">
-        <v>1366</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -3057,7 +3057,7 @@
         <v>2005</v>
       </c>
       <c r="C98">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -3090,7 +3090,7 @@
         <v>2020</v>
       </c>
       <c r="C101">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -3134,7 +3134,7 @@
         <v>2015</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -3145,7 +3145,7 @@
         <v>2020</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -3178,7 +3178,7 @@
         <v>2010</v>
       </c>
       <c r="C109">
-        <v>91.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -3211,7 +3211,7 @@
         <v>2000</v>
       </c>
       <c r="C112">
-        <v>735</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -3222,7 +3222,7 @@
         <v>2005</v>
       </c>
       <c r="C113">
-        <v>181</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -3288,7 +3288,7 @@
         <v>2010</v>
       </c>
       <c r="C119">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -3321,7 +3321,7 @@
         <v>2000</v>
       </c>
       <c r="C122">
-        <v>2418</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -3332,7 +3332,7 @@
         <v>2005</v>
       </c>
       <c r="C123">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -3343,7 +3343,7 @@
         <v>2010</v>
       </c>
       <c r="C124">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -3354,7 +3354,7 @@
         <v>2015</v>
       </c>
       <c r="C125">
-        <v>831</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -3365,7 +3365,7 @@
         <v>2020</v>
       </c>
       <c r="C126">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -3376,7 +3376,7 @@
         <v>2000</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -3387,7 +3387,7 @@
         <v>2005</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -3398,7 +3398,7 @@
         <v>2010</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>141</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -3409,7 +3409,7 @@
         <v>2015</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -3431,7 +3431,7 @@
         <v>2000</v>
       </c>
       <c r="C132">
-        <v>316</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -3453,7 +3453,7 @@
         <v>2010</v>
       </c>
       <c r="C134">
-        <v>140</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -3464,7 +3464,7 @@
         <v>2015</v>
       </c>
       <c r="C135">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -3475,7 +3475,7 @@
         <v>2020</v>
       </c>
       <c r="C136">
-        <v>93</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6528,7 +6528,7 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>3937</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -6539,7 +6539,7 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>27.63000000000011</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -6550,7 +6550,7 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>827.8900000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -6561,7 +6561,7 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>400.8699999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -6572,7 +6572,7 @@
         <v>2020</v>
       </c>
       <c r="C6">
-        <v>812.8899999999994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -6638,7 +6638,7 @@
         <v>2000</v>
       </c>
       <c r="C12">
-        <v>149</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -6693,7 +6693,7 @@
         <v>2000</v>
       </c>
       <c r="C17">
-        <v>275.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -6968,7 +6968,7 @@
         <v>2000</v>
       </c>
       <c r="C42">
-        <v>5408.63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -7012,7 +7012,7 @@
         <v>2020</v>
       </c>
       <c r="C46">
-        <v>85.59999999999945</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -7023,7 +7023,7 @@
         <v>2000</v>
       </c>
       <c r="C47">
-        <v>745</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -7034,7 +7034,7 @@
         <v>2005</v>
       </c>
       <c r="C48">
-        <v>331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -7045,7 +7045,7 @@
         <v>2010</v>
       </c>
       <c r="C49">
-        <v>53</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -7078,7 +7078,7 @@
         <v>2000</v>
       </c>
       <c r="C52">
-        <v>699</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -7243,7 +7243,7 @@
         <v>2000</v>
       </c>
       <c r="C67">
-        <v>3001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -7254,7 +7254,7 @@
         <v>2005</v>
       </c>
       <c r="C68">
-        <v>145</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -7265,7 +7265,7 @@
         <v>2010</v>
       </c>
       <c r="C69">
-        <v>157.6100000000001</v>
+        <v>4.72</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -7276,7 +7276,7 @@
         <v>2015</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1.350000000000001</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -7518,7 +7518,7 @@
         <v>2000</v>
       </c>
       <c r="C92">
-        <v>1326</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -7551,7 +7551,7 @@
         <v>2015</v>
       </c>
       <c r="C95">
-        <v>84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -7573,7 +7573,7 @@
         <v>2000</v>
       </c>
       <c r="C97">
-        <v>308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -7584,7 +7584,7 @@
         <v>2005</v>
       </c>
       <c r="C98">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -7595,7 +7595,7 @@
         <v>2010</v>
       </c>
       <c r="C99">
-        <v>2.949999999999989</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -7628,7 +7628,7 @@
         <v>2000</v>
       </c>
       <c r="C102">
-        <v>617</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -7639,7 +7639,7 @@
         <v>2005</v>
       </c>
       <c r="C103">
-        <v>431.9000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -7661,7 +7661,7 @@
         <v>2015</v>
       </c>
       <c r="C105">
-        <v>673.0999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -7672,7 +7672,7 @@
         <v>2020</v>
       </c>
       <c r="C106">
-        <v>1042.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -7716,7 +7716,7 @@
         <v>2015</v>
       </c>
       <c r="C110">
-        <v>278.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -7727,7 +7727,7 @@
         <v>2020</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -7848,7 +7848,7 @@
         <v>2000</v>
       </c>
       <c r="C122">
-        <v>2687</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -7870,7 +7870,7 @@
         <v>2010</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>732</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -7881,7 +7881,7 @@
         <v>2015</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>1572.01</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -7892,7 +7892,7 @@
         <v>2020</v>
       </c>
       <c r="C126">
-        <v>303</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -7947,7 +7947,7 @@
         <v>2020</v>
       </c>
       <c r="C131">
-        <v>99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -7958,7 +7958,7 @@
         <v>2000</v>
       </c>
       <c r="C132">
-        <v>9288</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -7969,7 +7969,7 @@
         <v>2005</v>
       </c>
       <c r="C133">
-        <v>62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -8002,7 +8002,7 @@
         <v>2020</v>
       </c>
       <c r="C136">
-        <v>1467</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8092,7 +8092,7 @@
         <v>2000</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -8125,7 +8125,7 @@
         <v>2015</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -8147,7 +8147,7 @@
         <v>2000</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>864</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -8257,7 +8257,7 @@
         <v>2000</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -8268,7 +8268,7 @@
         <v>2005</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -8290,7 +8290,7 @@
         <v>2015</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -8477,7 +8477,7 @@
         <v>2000</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>1727.66</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -8521,7 +8521,7 @@
         <v>2020</v>
       </c>
       <c r="C46">
-        <v>9</v>
+        <v>0.03999999999996362</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -8532,7 +8532,7 @@
         <v>2000</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>4654</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -8543,7 +8543,7 @@
         <v>2005</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>701</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -8554,7 +8554,7 @@
         <v>2010</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -8730,7 +8730,7 @@
         <v>2015</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>292</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -8752,7 +8752,7 @@
         <v>2000</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>3940.38</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -8774,7 +8774,7 @@
         <v>2010</v>
       </c>
       <c r="C69">
-        <v>4.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -8785,7 +8785,7 @@
         <v>2015</v>
       </c>
       <c r="C70">
-        <v>1.350000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -8862,7 +8862,7 @@
         <v>2000</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>760</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -8917,7 +8917,7 @@
         <v>2000</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -8950,7 +8950,7 @@
         <v>2015</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>196</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -9082,7 +9082,7 @@
         <v>2000</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -9093,7 +9093,7 @@
         <v>2005</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -9126,7 +9126,7 @@
         <v>2020</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -9214,7 +9214,7 @@
         <v>2010</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>91.5</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -9236,7 +9236,7 @@
         <v>2020</v>
       </c>
       <c r="C111">
-        <v>0.09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -9247,7 +9247,7 @@
         <v>2000</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>735</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -9258,7 +9258,7 @@
         <v>2005</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>181</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -9324,7 +9324,7 @@
         <v>2010</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -9357,7 +9357,7 @@
         <v>2000</v>
       </c>
       <c r="C122">
-        <v>0</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -9368,7 +9368,7 @@
         <v>2005</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -9379,7 +9379,7 @@
         <v>2010</v>
       </c>
       <c r="C124">
-        <v>732</v>
+        <v>25</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -9390,7 +9390,7 @@
         <v>2015</v>
       </c>
       <c r="C125">
-        <v>1572.01</v>
+        <v>831</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -9401,7 +9401,7 @@
         <v>2020</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -9467,7 +9467,7 @@
         <v>2000</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>316</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -9489,7 +9489,7 @@
         <v>2010</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>140</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -9500,7 +9500,7 @@
         <v>2015</v>
       </c>
       <c r="C135">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -9511,7 +9511,7 @@
         <v>2020</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -9546,7 +9546,7 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -9557,7 +9557,7 @@
         <v>2005</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>16.02</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -9568,7 +9568,7 @@
         <v>2010</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>67.8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -9579,7 +9579,7 @@
         <v>2015</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>848.28</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -9590,7 +9590,7 @@
         <v>2020</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -9612,7 +9612,7 @@
         <v>2005</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -9623,7 +9623,7 @@
         <v>2010</v>
       </c>
       <c r="C9">
-        <v>196.5</v>
+        <v>1004.6</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -9634,7 +9634,7 @@
         <v>2015</v>
       </c>
       <c r="C10">
-        <v>515.5</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -9645,7 +9645,7 @@
         <v>2020</v>
       </c>
       <c r="C11">
-        <v>1541.9</v>
+        <v>2514.8</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -9678,7 +9678,7 @@
         <v>2010</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -9689,7 +9689,7 @@
         <v>2015</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -9700,7 +9700,7 @@
         <v>2020</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>43.95000000000005</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -9733,7 +9733,7 @@
         <v>2010</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -9744,7 +9744,7 @@
         <v>2015</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -9755,7 +9755,7 @@
         <v>2020</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -9766,7 +9766,7 @@
         <v>2000</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -9777,7 +9777,7 @@
         <v>2005</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -9788,7 +9788,7 @@
         <v>2010</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1726.41</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -9799,7 +9799,7 @@
         <v>2015</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>346.4200000000001</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -9821,7 +9821,7 @@
         <v>2000</v>
       </c>
       <c r="C27">
-        <v>49.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -9832,7 +9832,7 @@
         <v>2005</v>
       </c>
       <c r="C28">
-        <v>373.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -9843,7 +9843,7 @@
         <v>2010</v>
       </c>
       <c r="C29">
-        <v>444.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -9854,7 +9854,7 @@
         <v>2015</v>
       </c>
       <c r="C30">
-        <v>403.1999999999999</v>
+        <v>775.11</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -9865,7 +9865,7 @@
         <v>2020</v>
       </c>
       <c r="C31">
-        <v>429.75</v>
+        <v>517.89</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -9898,7 +9898,7 @@
         <v>2010</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -9909,7 +9909,7 @@
         <v>2015</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -9920,7 +9920,7 @@
         <v>2020</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>123.8</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -9931,7 +9931,7 @@
         <v>2000</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -9942,7 +9942,7 @@
         <v>2005</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -9953,7 +9953,7 @@
         <v>2010</v>
       </c>
       <c r="C39">
-        <v>26.3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -9964,7 +9964,7 @@
         <v>2015</v>
       </c>
       <c r="C40">
-        <v>5.699999999999999</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -9975,7 +9975,7 @@
         <v>2020</v>
       </c>
       <c r="C41">
-        <v>41</v>
+        <v>374</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -9986,7 +9986,7 @@
         <v>2000</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -9997,7 +9997,7 @@
         <v>2005</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -10008,7 +10008,7 @@
         <v>2010</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -10019,7 +10019,7 @@
         <v>2015</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>6093.52</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -10030,7 +10030,7 @@
         <v>2020</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>4586.93</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -10041,7 +10041,7 @@
         <v>2000</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -10052,7 +10052,7 @@
         <v>2005</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -10063,7 +10063,7 @@
         <v>2010</v>
       </c>
       <c r="C49">
-        <v>80</v>
+        <v>15948</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -10074,7 +10074,7 @@
         <v>2015</v>
       </c>
       <c r="C50">
-        <v>3203</v>
+        <v>21218</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -10085,7 +10085,7 @@
         <v>2020</v>
       </c>
       <c r="C51">
-        <v>4464</v>
+        <v>14559</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -10107,7 +10107,7 @@
         <v>2005</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -10118,7 +10118,7 @@
         <v>2010</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -10129,7 +10129,7 @@
         <v>2015</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -10140,7 +10140,7 @@
         <v>2020</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>643</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -10173,7 +10173,7 @@
         <v>2010</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -10184,7 +10184,7 @@
         <v>2015</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -10195,7 +10195,7 @@
         <v>2020</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -10217,7 +10217,7 @@
         <v>2005</v>
       </c>
       <c r="C63">
-        <v>25.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -10228,7 +10228,7 @@
         <v>2010</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -10239,7 +10239,7 @@
         <v>2015</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -10250,7 +10250,7 @@
         <v>2020</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>37.84</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -10261,7 +10261,7 @@
         <v>2000</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -10272,7 +10272,7 @@
         <v>2005</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -10283,7 +10283,7 @@
         <v>2010</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>3558</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -10294,7 +10294,7 @@
         <v>2015</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>15309</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -10305,7 +10305,7 @@
         <v>2020</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>2693.279999999999</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -10349,7 +10349,7 @@
         <v>2015</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -10360,7 +10360,7 @@
         <v>2020</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -10393,7 +10393,7 @@
         <v>2010</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -10404,7 +10404,7 @@
         <v>2015</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>68.90000000000001</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -10415,7 +10415,7 @@
         <v>2020</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -10437,7 +10437,7 @@
         <v>2005</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>23.58</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -10448,7 +10448,7 @@
         <v>2010</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>5.870000000000001</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -10459,7 +10459,7 @@
         <v>2015</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>86.81999999999999</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -10470,7 +10470,7 @@
         <v>2020</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>78.47000000000001</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -10481,7 +10481,7 @@
         <v>2000</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -10492,7 +10492,7 @@
         <v>2005</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -10503,7 +10503,7 @@
         <v>2010</v>
       </c>
       <c r="C89">
-        <v>228</v>
+        <v>39</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -10514,7 +10514,7 @@
         <v>2015</v>
       </c>
       <c r="C90">
-        <v>129</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -10525,7 +10525,7 @@
         <v>2020</v>
       </c>
       <c r="C91">
-        <v>2143</v>
+        <v>8687</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -10536,7 +10536,7 @@
         <v>2000</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -10547,7 +10547,7 @@
         <v>2005</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -10558,7 +10558,7 @@
         <v>2010</v>
       </c>
       <c r="C94">
-        <v>2.3</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -10569,7 +10569,7 @@
         <v>2015</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -10580,7 +10580,7 @@
         <v>2020</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>136.7</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -10624,7 +10624,7 @@
         <v>2015</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>107.78</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -10635,7 +10635,7 @@
         <v>2020</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>3827.96</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -10646,7 +10646,7 @@
         <v>2000</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -10657,7 +10657,7 @@
         <v>2005</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -10668,7 +10668,7 @@
         <v>2010</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>132</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -10679,7 +10679,7 @@
         <v>2015</v>
       </c>
       <c r="C105">
-        <v>2</v>
+        <v>313</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -10690,7 +10690,7 @@
         <v>2020</v>
       </c>
       <c r="C106">
-        <v>23</v>
+        <v>578.4400000000001</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -10723,7 +10723,7 @@
         <v>2010</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -10734,7 +10734,7 @@
         <v>2015</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>1325.9</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -10745,7 +10745,7 @@
         <v>2020</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>60.71000000000004</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -10778,7 +10778,7 @@
         <v>2010</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -10789,7 +10789,7 @@
         <v>2015</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>514</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -10800,7 +10800,7 @@
         <v>2020</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>59.89999999999998</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -10811,7 +10811,7 @@
         <v>2000</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -10833,7 +10833,7 @@
         <v>2010</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -10844,7 +10844,7 @@
         <v>2015</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>226</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -10855,7 +10855,7 @@
         <v>2020</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>28.81</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -10866,7 +10866,7 @@
         <v>2000</v>
       </c>
       <c r="C122">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -10877,7 +10877,7 @@
         <v>2005</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -10888,7 +10888,7 @@
         <v>2010</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>3821</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -10899,7 +10899,7 @@
         <v>2015</v>
       </c>
       <c r="C125">
-        <v>5</v>
+        <v>831</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -10910,7 +10910,7 @@
         <v>2020</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>7081.01</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -10921,7 +10921,7 @@
         <v>2000</v>
       </c>
       <c r="C127">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -10932,7 +10932,7 @@
         <v>2005</v>
       </c>
       <c r="C128">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -10943,7 +10943,7 @@
         <v>2010</v>
       </c>
       <c r="C129">
-        <v>141</v>
+        <v>7</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -10954,7 +10954,7 @@
         <v>2015</v>
       </c>
       <c r="C130">
-        <v>40</v>
+        <v>93</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -10965,7 +10965,7 @@
         <v>2020</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>1313.15</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -10976,7 +10976,7 @@
         <v>2000</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -10987,7 +10987,7 @@
         <v>2005</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -10998,7 +10998,7 @@
         <v>2010</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>97</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -11009,7 +11009,7 @@
         <v>2015</v>
       </c>
       <c r="C135">
-        <v>0</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -11020,7 +11020,7 @@
         <v>2020</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>1549.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>